<commit_message>
Updated on Negative Testing
</commit_message>
<xml_diff>
--- a/TestData/PDF.xlsx
+++ b/TestData/PDF.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ADEC09-D6A6-4758-99D8-67954CEFE9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16230" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="PDFVALUES" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Project</t>
   </si>
@@ -31,41 +30,29 @@
     <t>ScreenShotsPath</t>
   </si>
   <si>
-    <t>C:\Users\91703\eclipse-workspace\pAInITe-master\test-output\Default suite\Default test.html</t>
-  </si>
-  <si>
-    <t>C:/Users/91703/eclipse-workspace/pAInITe-master/TestcaseScreenshots/</t>
-  </si>
-  <si>
-    <t>C:\Users\91703\eclipse-workspace\pAInITe-master\Logo\M10logo.png</t>
-  </si>
-  <si>
     <t>M10 Mlogo Path</t>
   </si>
   <si>
-    <t>C:\Users\91703\.jenkins\workspace\PDF\test-output\Default suite\Default test.html</t>
-  </si>
-  <si>
-    <t>HariKrishna</t>
-  </si>
-  <si>
-    <t>DataDriving</t>
-  </si>
-  <si>
-    <t>C:\Users\91703\eclipse-workspace\pAInITe-master\screenShots\</t>
-  </si>
-  <si>
-    <t>C:\Users\91703\.jenkins\workspace\PDF\screenShots\</t>
-  </si>
-  <si>
     <t xml:space="preserve">Key word driven </t>
   </si>
+  <si>
+    <t>C:\Users\Dell\Downloads\pAInITe-master\pAInITe-master\Logo\M10logo.png</t>
+  </si>
+  <si>
+    <t>C:/Users/Dell/Downloads/pAInITe-master/pAInITe-master/test-output/Default%20suite/Default%20test.html</t>
+  </si>
+  <si>
+    <t>Deepika</t>
+  </si>
+  <si>
+    <t>C:\Users\Dell\Downloads\pAInITe-master\pAInITe-master\TestcaseScreenshots\</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -119,6 +106,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -181,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,27 +203,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,24 +237,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -458,24 +412,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A6" sqref="A6:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.26953125" customWidth="1"/>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.08984375" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="26.1" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -489,47 +443,30 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -538,24 +475,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>